<commit_message>
Check at 0 ERRORs, 0 WARNINGs, 2 NOTEs. One NOTE for size, one NOTE for data documentation.
</commit_message>
<xml_diff>
--- a/inst/check_notes_20210318.xlsx
+++ b/inst/check_notes_20210318.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VAIO-PC\Documents\GitHub\coMethDMR\inst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/coMethDMR/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B57515E5-0FF8-4622-AC45-4D5F4EFE09D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2E98E0-DD07-D343-AF6B-038665CABB05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12168" xr2:uid="{43E2E1ED-674D-F442-BDA2-47771752FD3D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12160" xr2:uid="{43E2E1ED-674D-F442-BDA2-47771752FD3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t xml:space="preserve">Type </t>
   </si>
@@ -114,13 +114,19 @@
   </si>
   <si>
     <t>change the files names to vin1 and vin2</t>
+  </si>
+  <si>
+    <t>enhancer.probes.Rd:10-12: Dropping empty section \source</t>
+  </si>
+  <si>
+    <t>regions.Rd:13-15: Dropping empty section \source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -486,20 +492,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82472AF-BD71-E040-97DF-AD406FB9C20A}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="73.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.69921875" customWidth="1"/>
+    <col min="2" max="2" width="73.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -521,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -535,7 +541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -546,7 +552,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -557,7 +563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -569,7 +575,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -581,7 +587,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -595,7 +601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -609,7 +615,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -621,6 +627,22 @@
       </c>
       <c r="D10" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>